<commit_message>
DB updation working. Testing API.
</commit_message>
<xml_diff>
--- a/Inputs/City_Geospatial_Data.xlsx
+++ b/Inputs/City_Geospatial_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bayer\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F79F2D-2F03-4131-A1E2-3DCA1A7989F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEF393B-5E51-4AED-8E67-38B5822E687F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{985C179B-B4DC-4D0D-BBEA-36EB6A3044FC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>City</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Centralia</t>
-  </si>
-  <si>
-    <t>Hebron</t>
   </si>
   <si>
     <t>Illipolis</t>
@@ -493,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC99EBF-76CD-4539-AEE3-1D372F5D8545}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,7 +574,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>40.1387</v>
@@ -608,13 +605,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>40.0916</v>
+        <v>39.758200000000002</v>
       </c>
       <c r="C8">
-        <v>-82.483099999999993</v>
+        <v>-89.658900000000003</v>
       </c>
       <c r="D8" s="3">
-        <v>1060</v>
+        <v>604</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -622,13 +619,13 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>39.758200000000002</v>
+        <v>39.008499999999998</v>
       </c>
       <c r="C9">
-        <v>-89.658900000000003</v>
+        <v>-94.346100000000007</v>
       </c>
       <c r="D9" s="3">
-        <v>604</v>
+        <v>856</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -636,13 +633,13 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>39.008499999999998</v>
+        <v>40.855200000000004</v>
       </c>
       <c r="C10">
-        <v>-94.346100000000007</v>
+        <v>-99.075000000000003</v>
       </c>
       <c r="D10" s="3">
-        <v>856</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -650,13 +647,13 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>40.855200000000004</v>
+        <v>29.9132</v>
       </c>
       <c r="C11">
-        <v>-99.075000000000003</v>
+        <v>-90.358099999999993</v>
       </c>
       <c r="D11" s="3">
-        <v>2254</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -664,13 +661,13 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>29.9132</v>
+        <v>40.9617</v>
       </c>
       <c r="C12">
-        <v>-90.358099999999993</v>
+        <v>-74.078199999999995</v>
       </c>
       <c r="D12" s="3">
-        <v>3</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -678,41 +675,41 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>40.9617</v>
+        <v>41.483899999999998</v>
       </c>
       <c r="C13">
-        <v>-74.078199999999995</v>
+        <v>-91.112799999999993</v>
       </c>
       <c r="D13" s="3">
-        <v>66</v>
+        <v>663</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B14">
-        <v>41.483899999999998</v>
+        <v>40.367199999999997</v>
       </c>
       <c r="C14">
-        <v>-91.112799999999993</v>
+        <v>-76.457700000000003</v>
       </c>
       <c r="D14" s="3">
-        <v>663</v>
+        <v>564</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>40.367199999999997</v>
+        <v>33.3489</v>
       </c>
       <c r="C15">
-        <v>-76.457700000000003</v>
+        <v>-112.49120000000001</v>
       </c>
       <c r="D15" s="3">
-        <v>564</v>
+        <v>909</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -720,13 +717,13 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>33.3489</v>
+        <v>40.468800000000002</v>
       </c>
       <c r="C16">
-        <v>-112.49120000000001</v>
+        <v>-79.981200000000001</v>
       </c>
       <c r="D16" s="3">
-        <v>909</v>
+        <v>886</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -734,13 +731,13 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>40.468800000000002</v>
+        <v>41.023000000000003</v>
       </c>
       <c r="C17">
-        <v>-79.981200000000001</v>
+        <v>-87.116200000000006</v>
       </c>
       <c r="D17" s="3">
-        <v>886</v>
+        <v>692</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -748,13 +745,13 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>41.023000000000003</v>
+        <v>36.339199999999998</v>
       </c>
       <c r="C18">
-        <v>-87.116200000000006</v>
+        <v>-94.257400000000004</v>
       </c>
       <c r="D18" s="3">
-        <v>692</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -762,13 +759,13 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>36.339199999999998</v>
+        <v>37.755699999999997</v>
       </c>
       <c r="C19">
-        <v>-94.257400000000004</v>
+        <v>-122.44280000000001</v>
       </c>
       <c r="D19" s="3">
-        <v>1257</v>
+        <v>472</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -776,13 +773,13 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>37.755699999999997</v>
+        <v>44.648600000000002</v>
       </c>
       <c r="C20">
-        <v>-122.44280000000001</v>
+        <v>-93.535399999999996</v>
       </c>
       <c r="D20" s="3">
-        <v>472</v>
+        <v>958</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -790,13 +787,13 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>44.648600000000002</v>
+        <v>32.0974</v>
       </c>
       <c r="C21">
-        <v>-93.535399999999996</v>
+        <v>-111.7899</v>
       </c>
       <c r="D21" s="3">
-        <v>958</v>
+        <v>3310</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -804,13 +801,13 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>32.0974</v>
+        <v>41.893500000000003</v>
       </c>
       <c r="C22">
-        <v>-111.7899</v>
+        <v>-88.770300000000006</v>
       </c>
       <c r="D22" s="3">
-        <v>3310</v>
+        <v>883</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -818,13 +815,13 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>41.893500000000003</v>
+        <v>40.862000000000002</v>
       </c>
       <c r="C23">
-        <v>-88.770300000000006</v>
+        <v>-74.544399999999996</v>
       </c>
       <c r="D23" s="3">
-        <v>883</v>
+        <v>650</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -832,30 +829,17 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>40.862000000000002</v>
+        <v>38.686700000000002</v>
       </c>
       <c r="C24">
-        <v>-74.544399999999996</v>
+        <v>-121.90170000000001</v>
       </c>
       <c r="D24" s="3">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25">
-        <v>38.686700000000002</v>
-      </c>
-      <c r="C25">
-        <v>-121.90170000000001</v>
-      </c>
-      <c r="D25" s="3">
         <v>128</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated dashboard and code
</commit_message>
<xml_diff>
--- a/Inputs/City_Geospatial_Data.xlsx
+++ b/Inputs/City_Geospatial_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bayer\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEF393B-5E51-4AED-8E67-38B5822E687F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB17B32-6606-4867-AD39-014B56EB7EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{985C179B-B4DC-4D0D-BBEA-36EB6A3044FC}"/>
+    <workbookView xWindow="4848" yWindow="1632" windowWidth="17280" windowHeight="8880" xr2:uid="{985C179B-B4DC-4D0D-BBEA-36EB6A3044FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>City</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Myerstown</t>
+  </si>
+  <si>
+    <t>Hebron</t>
   </si>
 </sst>
 </file>
@@ -166,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -176,6 +179,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,19 +495,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC99EBF-76CD-4539-AEE3-1D372F5D8545}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,8 +521,9 @@
       <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -530,7 +537,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -544,7 +551,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -558,7 +565,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -572,7 +579,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -586,7 +593,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -600,241 +607,255 @@
         <v>620</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>42.324399999999997</v>
+      </c>
+      <c r="C8">
+        <v>-88.452399999999997</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>39.758200000000002</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>-89.658900000000003</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="3">
         <v>604</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>39.008499999999998</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>-94.346100000000007</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D10" s="3">
         <v>856</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>40.855200000000004</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>-99.075000000000003</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D11" s="3">
         <v>2254</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>29.9132</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>-90.358099999999993</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D12" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>40.9617</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>-74.078199999999995</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D13" s="3">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>41.483899999999998</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>-91.112799999999993</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D14" s="3">
         <v>663</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>40.367199999999997</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>-76.457700000000003</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D15" s="3">
         <v>564</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>33.3489</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>-112.49120000000001</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D16" s="3">
         <v>909</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>40.468800000000002</v>
-      </c>
-      <c r="C16">
-        <v>-79.981200000000001</v>
-      </c>
-      <c r="D16" s="3">
-        <v>886</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>41.023000000000003</v>
+        <v>40.468800000000002</v>
       </c>
       <c r="C17">
-        <v>-87.116200000000006</v>
+        <v>-79.981200000000001</v>
       </c>
       <c r="D17" s="3">
-        <v>692</v>
+        <v>886</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>36.339199999999998</v>
+        <v>41.023000000000003</v>
       </c>
       <c r="C18">
-        <v>-94.257400000000004</v>
+        <v>-87.116200000000006</v>
       </c>
       <c r="D18" s="3">
-        <v>1257</v>
+        <v>692</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>37.755699999999997</v>
+        <v>36.339199999999998</v>
       </c>
       <c r="C19">
-        <v>-122.44280000000001</v>
+        <v>-94.257400000000004</v>
       </c>
       <c r="D19" s="3">
-        <v>472</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>44.648600000000002</v>
+        <v>37.755699999999997</v>
       </c>
       <c r="C20">
-        <v>-93.535399999999996</v>
+        <v>-122.44280000000001</v>
       </c>
       <c r="D20" s="3">
-        <v>958</v>
+        <v>472</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>32.0974</v>
+        <v>44.648600000000002</v>
       </c>
       <c r="C21">
-        <v>-111.7899</v>
+        <v>-93.535399999999996</v>
       </c>
       <c r="D21" s="3">
-        <v>3310</v>
+        <v>958</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>41.893500000000003</v>
+        <v>32.0974</v>
       </c>
       <c r="C22">
-        <v>-88.770300000000006</v>
+        <v>-111.7899</v>
       </c>
       <c r="D22" s="3">
-        <v>883</v>
+        <v>3310</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>40.862000000000002</v>
+        <v>41.893500000000003</v>
       </c>
       <c r="C23">
-        <v>-74.544399999999996</v>
+        <v>-88.770300000000006</v>
       </c>
       <c r="D23" s="3">
-        <v>650</v>
+        <v>883</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>40.862000000000002</v>
+      </c>
+      <c r="C24">
+        <v>-74.544399999999996</v>
+      </c>
+      <c r="D24" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>38.686700000000002</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>-121.90170000000001</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D25" s="3">
         <v>128</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added additional data for dashboarding
</commit_message>
<xml_diff>
--- a/Inputs/City_Geospatial_Data.xlsx
+++ b/Inputs/City_Geospatial_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bayer\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB17B32-6606-4867-AD39-014B56EB7EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777B53EB-0DC1-425C-8976-C638FA951CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4848" yWindow="1632" windowWidth="17280" windowHeight="8880" xr2:uid="{985C179B-B4DC-4D0D-BBEA-36EB6A3044FC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{985C179B-B4DC-4D0D-BBEA-36EB6A3044FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>City</t>
   </si>
@@ -120,6 +120,72 @@
   </si>
   <si>
     <t>Hebron</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>Lorain</t>
+  </si>
+  <si>
+    <t>Alameda</t>
+  </si>
+  <si>
+    <t>Middlesex</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>St. Louis</t>
+  </si>
+  <si>
+    <t>Licking</t>
+  </si>
+  <si>
+    <t>Sangamon</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>Caldwell</t>
+  </si>
+  <si>
+    <t>Bergen</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Maricopa</t>
+  </si>
+  <si>
+    <t>Alleghany</t>
+  </si>
+  <si>
+    <t>Jasper</t>
+  </si>
+  <si>
+    <t>Benton</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Pima</t>
+  </si>
+  <si>
+    <t>DeKalb</t>
+  </si>
+  <si>
+    <t>Morris</t>
+  </si>
+  <si>
+    <t>Yolo</t>
   </si>
 </sst>
 </file>
@@ -169,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -179,8 +245,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,15 +561,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC99EBF-76CD-4539-AEE3-1D372F5D8545}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -521,7 +585,9 @@
       <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -536,6 +602,9 @@
       <c r="D2" s="3">
         <v>771</v>
       </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -550,6 +619,9 @@
       <c r="D3" s="3">
         <v>358</v>
       </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -564,6 +636,9 @@
       <c r="D4" s="3">
         <v>194</v>
       </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -573,10 +648,13 @@
         <v>38.6496</v>
       </c>
       <c r="C5">
-        <v>-88.918999999999997</v>
+        <v>-89.410600000000002</v>
       </c>
       <c r="D5" s="3">
         <v>561</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -584,13 +662,16 @@
         <v>25</v>
       </c>
       <c r="B6">
-        <v>40.1387</v>
+        <v>40.140099999999997</v>
       </c>
       <c r="C6">
-        <v>-88.251599999999996</v>
+        <v>-88.199200000000005</v>
       </c>
       <c r="D6" s="3">
         <v>748</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -606,19 +687,25 @@
       <c r="D7" s="3">
         <v>620</v>
       </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
       <c r="B8">
-        <v>42.324399999999997</v>
+        <v>40.0916</v>
       </c>
       <c r="C8">
-        <v>-88.452399999999997</v>
+        <v>-82.483099999999993</v>
       </c>
       <c r="D8" s="3">
         <v>1060</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -634,6 +721,9 @@
       <c r="D9" s="3">
         <v>604</v>
       </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -648,6 +738,9 @@
       <c r="D10" s="3">
         <v>856</v>
       </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -662,19 +755,25 @@
       <c r="D11" s="3">
         <v>2254</v>
       </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
-        <v>29.9132</v>
+        <v>32.092300000000002</v>
       </c>
       <c r="C12">
-        <v>-90.358099999999993</v>
+        <v>-92.116600000000005</v>
       </c>
       <c r="D12" s="3">
         <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -690,6 +789,9 @@
       <c r="D13" s="3">
         <v>66</v>
       </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -704,6 +806,9 @@
       <c r="D14" s="3">
         <v>663</v>
       </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -718,6 +823,9 @@
       <c r="D15" s="3">
         <v>564</v>
       </c>
+      <c r="E15" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -732,8 +840,11 @@
       <c r="D16" s="3">
         <v>909</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -746,8 +857,11 @@
       <c r="D17" s="3">
         <v>886</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -760,8 +874,11 @@
       <c r="D18" s="3">
         <v>692</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -774,8 +891,11 @@
       <c r="D19" s="3">
         <v>1257</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -789,7 +909,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -802,8 +922,11 @@
       <c r="D21" s="3">
         <v>958</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -816,8 +939,11 @@
       <c r="D22" s="3">
         <v>3310</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -830,8 +956,11 @@
       <c r="D23" s="3">
         <v>883</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -844,8 +973,11 @@
       <c r="D24" s="3">
         <v>650</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -857,6 +989,9 @@
       </c>
       <c r="D25" s="3">
         <v>128</v>
+      </c>
+      <c r="E25" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>